<commit_message>
Ahora no lo borres.xls actualizado
</commit_message>
<xml_diff>
--- a/Ahora no lo borres.xlsx
+++ b/Ahora no lo borres.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ProyectoR\Desktop\MiProyectoVespertino2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristofher\Desktop\MiProyectoVespertino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01A7BE0-6BEE-408A-999B-F7C3F01C7151}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D23A60-3F82-46B3-B215-5FCB6632ACD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24345" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>2+2=4</t>
+  </si>
+  <si>
+    <t>2+3=5</t>
   </si>
 </sst>
 </file>
@@ -345,7 +348,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -358,6 +361,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>